<commit_message>
Atualizando os dados , Modificando o para_km para 1247954.666
</commit_message>
<xml_diff>
--- a/Impacto Econômico do Milho, Soja e Pecuária no Desmatamento no Pará/Produção de Milho(R$)-km + desmatamento(Pará).xlsx
+++ b/Impacto Econômico do Milho, Soja e Pecuária no Desmatamento no Pará/Produção de Milho(R$)-km + desmatamento(Pará).xlsx
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.2290623919464598</v>
+        <v>0.2300186582838494</v>
       </c>
     </row>
     <row r="3">
@@ -484,7 +484,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.2220645348485394</v>
+        <v>0.222991587245047</v>
       </c>
     </row>
     <row r="4">
@@ -500,7 +500,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.2000189360963008</v>
+        <v>0.2008539547731077</v>
       </c>
     </row>
     <row r="5">
@@ -516,7 +516,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.2167336017514379</v>
+        <v>0.2176383991115586</v>
       </c>
     </row>
     <row r="6">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.3061667294050382</v>
+        <v>0.3074448830751838</v>
       </c>
     </row>
     <row r="7">
@@ -548,7 +548,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.2836849957085151</v>
+        <v>0.2848692949272273</v>
       </c>
     </row>
     <row r="8">
@@ -564,7 +564,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.2292412064481024</v>
+        <v>0.2301982192820561</v>
       </c>
     </row>
     <row r="9">
@@ -580,7 +580,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.2279081942084092</v>
+        <v>0.2288596421186697</v>
       </c>
     </row>
     <row r="10">
@@ -596,7 +596,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.1057664978470095</v>
+        <v>0.1062080410469003</v>
       </c>
     </row>
     <row r="11">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.1070922748913763</v>
+        <v>0.1075393528102039</v>
       </c>
     </row>
     <row r="12">
@@ -628,7 +628,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.1096731963456842</v>
+        <v>0.1101310488324591</v>
       </c>
     </row>
     <row r="13">
@@ -644,7 +644,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.09093133797656133</v>
+        <v>0.09131094886240723</v>
       </c>
     </row>
     <row r="14">
@@ -660,7 +660,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.2167620458514672</v>
+        <v>0.2176669619571188</v>
       </c>
     </row>
     <row r="15">
@@ -676,7 +676,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.2110438622937427</v>
+        <v>0.2119249067092369</v>
       </c>
     </row>
     <row r="16">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.2227039054285122</v>
+        <v>0.223633627004179</v>
       </c>
     </row>
     <row r="17">
@@ -708,7 +708,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.1802776466792893</v>
+        <v>0.1810302514322489</v>
       </c>
     </row>
     <row r="18">
@@ -724,7 +724,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.2127854441957589</v>
+        <v>0.2136737591899481</v>
       </c>
     </row>
     <row r="19">
@@ -740,7 +740,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.2323160969779649</v>
+        <v>0.2332859465516377</v>
       </c>
     </row>
     <row r="20">
@@ -756,7 +756,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.2095693773981687</v>
+        <v>0.2104442662843391</v>
       </c>
     </row>
     <row r="21">
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.2101126205874776</v>
+        <v>0.2109897773499699</v>
       </c>
     </row>
     <row r="22">
@@ -788,7 +788,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.211761430609176</v>
+        <v>0.2126454706557688</v>
       </c>
     </row>
     <row r="23">
@@ -804,7 +804,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.2768646765800862</v>
+        <v>0.2780205030253442</v>
       </c>
     </row>
   </sheetData>

</xml_diff>